<commit_message>
Embebido, PWA , Gestión y Protocolos
1.- Embebido:
1.1.- Mejoras en el manejo de los tiempos
2.- PWA:
2.1.- Se agregó límite de velocidad
3.- Gestión:
3.1.- Excel de facturación
3.2.- Excel de actualización de equipos
4.- Protocolos:
4.1.- Protocolo de instalación
</commit_message>
<xml_diff>
--- a/Control de equipos.xlsx
+++ b/Control de equipos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L03502024\Documents\GitHub\dta-agricola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AA8C40-CEE4-4492-B686-24FBA00F9C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DC6EF4-28FB-469D-93DA-70AE93ECBFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" tabRatio="484" xr2:uid="{81E9D037-BE23-435E-B775-5A4C621A153A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="458" xr2:uid="{81E9D037-BE23-435E-B775-5A4C621A153A}"/>
   </bookViews>
   <sheets>
     <sheet name="Control de equipos" sheetId="8" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Hoja3" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="132">
   <si>
     <t>Equipo</t>
   </si>
@@ -207,9 +208,6 @@
     <t>8952020020333844270</t>
   </si>
   <si>
-    <t>JQC12V-0</t>
-  </si>
-  <si>
     <t>GPS</t>
   </si>
   <si>
@@ -219,24 +217,6 @@
     <t>Alias</t>
   </si>
   <si>
-    <t>P1996</t>
-  </si>
-  <si>
-    <t>P9145</t>
-  </si>
-  <si>
-    <t>P0168</t>
-  </si>
-  <si>
-    <t>P7317</t>
-  </si>
-  <si>
-    <t>P2314</t>
-  </si>
-  <si>
-    <t>P9200</t>
-  </si>
-  <si>
     <t>Johan L3</t>
   </si>
   <si>
@@ -261,9 +241,6 @@
     <t>Johan L12</t>
   </si>
   <si>
-    <t>Claudio</t>
-  </si>
-  <si>
     <t>Claudio P1</t>
   </si>
   <si>
@@ -309,26 +286,161 @@
     <t>8952020020633586704</t>
   </si>
   <si>
-    <t>P0790</t>
-  </si>
-  <si>
     <t>8952020020633586688</t>
   </si>
   <si>
-    <t>P0232</t>
-  </si>
-  <si>
-    <t>P2598</t>
-  </si>
-  <si>
     <t>Pv66 v0.2.4.0 A</t>
+  </si>
+  <si>
+    <t>Knals L21</t>
+  </si>
+  <si>
+    <t>Cornelio Wibe</t>
+  </si>
+  <si>
+    <t>Johan Krahn</t>
+  </si>
+  <si>
+    <t>Bernardo Krahn</t>
+  </si>
+  <si>
+    <t>Claudio González</t>
+  </si>
+  <si>
+    <t>Abraham 4</t>
+  </si>
+  <si>
+    <t>Abraham</t>
+  </si>
+  <si>
+    <t>Valley</t>
+  </si>
+  <si>
+    <t>Zimmatic</t>
+  </si>
+  <si>
+    <t>Reinke</t>
+  </si>
+  <si>
+    <t>Abraham 1</t>
+  </si>
+  <si>
+    <t>Abraham 7</t>
+  </si>
+  <si>
+    <t>Reintic</t>
+  </si>
+  <si>
+    <t>Abraham 8</t>
+  </si>
+  <si>
+    <t>FL-0</t>
+  </si>
+  <si>
+    <t>Pv66-A</t>
+  </si>
+  <si>
+    <t>Pv66 v0.2.4.220403 A</t>
+  </si>
+  <si>
+    <t>[Latitud,Longitud]</t>
+  </si>
+  <si>
+    <t>Tipo/Marca</t>
+  </si>
+  <si>
+    <t>[30.73081,-107.86308]</t>
+  </si>
+  <si>
+    <t>[,]</t>
+  </si>
+  <si>
+    <t>[31.1682,-108.224705]</t>
+  </si>
+  <si>
+    <t>[31.168301,-108.23546]</t>
+  </si>
+  <si>
+    <t>[31.177465,-108.214081]</t>
+  </si>
+  <si>
+    <t>[31.177441,-108.224663]</t>
+  </si>
+  <si>
+    <t>[31.186665,-108.214106]</t>
+  </si>
+  <si>
+    <t>[31.1275895,-108.18300125]</t>
+  </si>
+  <si>
+    <t>[30.727967,-107.894213]</t>
+  </si>
+  <si>
+    <t>[28.407219,-106.863445]</t>
+  </si>
+  <si>
+    <t>[30.73537,-107.89424]</t>
+  </si>
+  <si>
+    <t>Knals L19</t>
+  </si>
+  <si>
+    <t>[28.422067,-107.51106]</t>
+  </si>
+  <si>
+    <t>[30.922254,-108.543824]</t>
+  </si>
+  <si>
+    <t>[30.95348,-108.520523]</t>
+  </si>
+  <si>
+    <t>El cable de pistola no llega a la última torre. Se invirtieron los cables de seguridad Amarillo-Rojo y Amarillo. Se sensa la seguridad en el Amarillo.</t>
+  </si>
+  <si>
+    <t>34/28</t>
+  </si>
+  <si>
+    <t>36/30</t>
+  </si>
+  <si>
+    <t>Pv66 v0.2.4.220412 A</t>
+  </si>
+  <si>
+    <t>[30.74075,-107.867944]</t>
+  </si>
+  <si>
+    <t>JQC12V-1</t>
+  </si>
+  <si>
+    <t>1745/1425 (~42rpm)</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
+  <si>
+    <t>Límite máximo de 80% para evitar torcedura, debido a que el penúltimo motor es de Baja y no puede seguir el ritmo del último | Seguridad se corta constantemente y espera 3 min para conectarse nuevamente</t>
+  </si>
+  <si>
+    <t>Relay de 4 canales: Tout tiene 110V fijos</t>
+  </si>
+  <si>
+    <t>Pv66 v0.2.4.220414 A</t>
+  </si>
+  <si>
+    <t>Abraham 5</t>
+  </si>
+  <si>
+    <t>[30.725965,-107.874697]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,8 +469,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,6 +501,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -444,59 +589,193 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -812,701 +1091,943 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07BF86A-6972-496C-8446-0DD77854D911}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.08984375" style="21" customWidth="1"/>
-    <col min="2" max="2" width="20.08984375" style="21" customWidth="1"/>
-    <col min="3" max="3" width="13.36328125" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" style="21" customWidth="1"/>
-    <col min="5" max="6" width="11.54296875" style="21"/>
-    <col min="7" max="7" width="14" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.54296875" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.54296875" style="21"/>
-    <col min="10" max="10" width="19.1796875" style="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="19.1796875" style="21" customWidth="1"/>
-    <col min="13" max="13" width="36.453125" style="21" customWidth="1"/>
-    <col min="14" max="16384" width="11.54296875" style="21"/>
+    <col min="1" max="1" width="5.08984375" style="33" customWidth="1"/>
+    <col min="2" max="2" width="21.36328125" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" style="33" customWidth="1"/>
+    <col min="5" max="6" width="11.54296875" style="33"/>
+    <col min="7" max="7" width="19.453125" style="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.54296875" style="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.36328125" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.26953125" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.08984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="19.1796875" style="33" customWidth="1"/>
+    <col min="15" max="15" width="36.453125" style="53" customWidth="1"/>
+    <col min="16" max="23" width="12.1796875" style="37" customWidth="1"/>
+    <col min="24" max="16384" width="11.54296875" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="O1" s="81" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="81"/>
+      <c r="T1" s="81"/>
+      <c r="U1" s="81"/>
+      <c r="V1" s="81"/>
+      <c r="W1" s="81"/>
+    </row>
+    <row r="2" spans="1:23" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B2" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C2" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="P2" s="19">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="19">
+        <v>2</v>
+      </c>
+      <c r="R2" s="19">
+        <v>3</v>
+      </c>
+      <c r="S2" s="19">
+        <v>4</v>
+      </c>
+      <c r="T2" s="19">
+        <v>5</v>
+      </c>
+      <c r="U2" s="19">
+        <v>6</v>
+      </c>
+      <c r="V2" s="19">
+        <v>7</v>
+      </c>
+      <c r="W2" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="23">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="25">
+        <v>526251106286</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="27">
+        <v>1211</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" s="23"/>
+      <c r="L3" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="M3" s="30">
+        <v>43872</v>
+      </c>
+      <c r="N3" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="O3" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58"/>
+      <c r="W3" s="58"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4" s="33">
         <v>2</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="B4" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="35">
+        <v>526251271378</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="36">
+        <v>1211</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="L4" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="M4" s="40">
+        <v>44603</v>
+      </c>
+      <c r="N4" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="O4" s="41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A5" s="42">
+        <v>3</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="35">
+        <v>526251024489</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="36">
+        <v>1211</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="M5" s="40">
+        <v>44603</v>
+      </c>
+      <c r="N5" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="O5" s="41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A6" s="33">
+        <v>4</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="35">
+        <v>526251452797</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="36">
+        <v>1211</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="J6" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="L6" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="M6" s="40">
+        <v>44603</v>
+      </c>
+      <c r="N6" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="O6" s="41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A7" s="42">
+        <v>5</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="35">
+        <v>526255917395</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="36">
+        <v>1211</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="M7" s="40">
+        <v>44603</v>
+      </c>
+      <c r="N7" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="O7" s="41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A8" s="33">
+        <v>6</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="35">
+        <v>526251193016</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="36">
+        <v>1211</v>
+      </c>
+      <c r="G8" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="J8" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="M8" s="40">
+        <v>44603</v>
+      </c>
+      <c r="N8" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="O8" s="41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A9" s="42">
+        <v>7</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="35">
+        <v>526251579804</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="36">
+        <v>1211</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="J9" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="42"/>
+      <c r="L9" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="M9" s="40">
+        <v>44603</v>
+      </c>
+      <c r="N9" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="O9" s="41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="33">
+        <v>8</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="44">
+        <v>526251201079</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="46">
+        <v>1211</v>
+      </c>
+      <c r="G10" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="H10" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="J10" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="48"/>
+      <c r="L10" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="M10" s="49">
+        <v>44384</v>
+      </c>
+      <c r="N10" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="O10" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="56"/>
+      <c r="S10" s="56"/>
+      <c r="T10" s="56"/>
+      <c r="U10" s="56"/>
+      <c r="V10" s="56"/>
+      <c r="W10" s="56"/>
+    </row>
+    <row r="11" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="59">
+        <v>9</v>
+      </c>
+      <c r="B11" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="61">
+        <v>526258372598</v>
+      </c>
+      <c r="D11" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="62">
+        <v>1211</v>
+      </c>
+      <c r="G11" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="H11" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="J11" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="K11" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="L11" s="70" t="s">
+        <v>131</v>
+      </c>
+      <c r="M11" s="66">
+        <v>44646</v>
+      </c>
+      <c r="N11" s="65"/>
+      <c r="O11" s="79"/>
+      <c r="P11" s="69"/>
+      <c r="Q11" s="69"/>
+      <c r="R11" s="69"/>
+      <c r="S11" s="69"/>
+      <c r="T11" s="69"/>
+      <c r="U11" s="69"/>
+      <c r="V11" s="69"/>
+      <c r="W11" s="69"/>
+    </row>
+    <row r="12" spans="1:23" s="59" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A12" s="59">
+        <v>10</v>
+      </c>
+      <c r="B12" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="61">
+        <v>526251531996</v>
+      </c>
+      <c r="D12" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="62">
+        <v>1211</v>
+      </c>
+      <c r="G12" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="H12" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="J12" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="K12" s="65" t="s">
+        <v>91</v>
+      </c>
+      <c r="L12" s="70" t="s">
+        <v>113</v>
+      </c>
+      <c r="M12" s="70"/>
+      <c r="N12" s="65"/>
+      <c r="O12" s="80" t="s">
+        <v>127</v>
+      </c>
+      <c r="P12" s="69"/>
+      <c r="Q12" s="69"/>
+      <c r="R12" s="69"/>
+      <c r="S12" s="69"/>
+      <c r="T12" s="69"/>
+      <c r="U12" s="69"/>
+      <c r="V12" s="69"/>
+      <c r="W12" s="69"/>
+    </row>
+    <row r="13" spans="1:23" s="59" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="59">
+        <v>11</v>
+      </c>
+      <c r="B13" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="61">
+        <v>526251259145</v>
+      </c>
+      <c r="D13" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="62">
+        <v>1211</v>
+      </c>
+      <c r="G13" s="78" t="s">
+        <v>121</v>
+      </c>
+      <c r="H13" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="J13" s="65" t="s">
+        <v>95</v>
+      </c>
+      <c r="K13" s="65" t="s">
+        <v>91</v>
+      </c>
+      <c r="L13" s="66" t="s">
+        <v>103</v>
+      </c>
+      <c r="M13" s="66">
+        <v>44662</v>
+      </c>
+      <c r="N13" s="65"/>
+      <c r="O13" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="P13" s="68" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q13" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="R13" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="S13" s="69" t="s">
+        <v>119</v>
+      </c>
+      <c r="T13" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="U13" s="69" t="s">
+        <v>57</v>
+      </c>
+      <c r="V13" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="W13" s="69" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A14" s="33">
+        <v>12</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="35">
+        <v>526251060168</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="36">
+        <v>1211</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="H14" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="M14" s="52"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="72"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A15" s="42">
+        <v>13</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="35">
+        <v>526251342314</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="36">
+        <v>1211</v>
+      </c>
+      <c r="G15" s="77" t="s">
+        <v>121</v>
+      </c>
+      <c r="H15" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="M15" s="39">
+        <v>44646</v>
+      </c>
+      <c r="N15" s="51"/>
+      <c r="O15" s="76" t="s">
+        <v>128</v>
+      </c>
+      <c r="P15" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q15" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="R15" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="S15" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="T15" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="U15" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="V15" s="75" t="s">
+        <v>126</v>
+      </c>
+      <c r="W15" s="37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="59">
+        <v>14</v>
+      </c>
+      <c r="B16" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="61">
+        <v>526251037317</v>
+      </c>
+      <c r="D16" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="62">
+        <v>1312</v>
+      </c>
+      <c r="G16" s="78" t="s">
+        <v>121</v>
+      </c>
+      <c r="H16" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="J16" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="K16" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="L16" s="70" t="s">
+        <v>122</v>
+      </c>
+      <c r="M16" s="66">
+        <v>44646</v>
+      </c>
+      <c r="N16" s="65"/>
+      <c r="O16" s="71"/>
+      <c r="P16" s="69"/>
+      <c r="Q16" s="69"/>
+      <c r="R16" s="69"/>
+      <c r="S16" s="69"/>
+      <c r="T16" s="69"/>
+      <c r="U16" s="69"/>
+      <c r="V16" s="69"/>
+      <c r="W16" s="69"/>
+    </row>
+    <row r="17" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="59">
+        <v>15</v>
+      </c>
+      <c r="B17" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="73">
+        <v>526251020232</v>
+      </c>
+      <c r="D17" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="69">
+        <v>1312</v>
+      </c>
+      <c r="G17" s="78" t="s">
+        <v>121</v>
+      </c>
+      <c r="H17" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="I17" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="J17" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="K17" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="L17" s="66" t="s">
+        <v>111</v>
+      </c>
+      <c r="M17" s="70"/>
+      <c r="O17" s="74"/>
+      <c r="P17" s="69"/>
+      <c r="Q17" s="69"/>
+      <c r="R17" s="69"/>
+      <c r="S17" s="69"/>
+      <c r="T17" s="69"/>
+      <c r="U17" s="69"/>
+      <c r="V17" s="69"/>
+      <c r="W17" s="69"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A18" s="33">
+        <v>16</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="35">
+        <v>526251059200</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18" s="36">
+        <v>1211</v>
+      </c>
+      <c r="G18" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="H18" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="J18" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="21">
-        <v>1</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="23">
-        <v>526251271378</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="24" t="s">
+      <c r="K18" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="L18" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="M18" s="39">
+        <v>44647</v>
+      </c>
+      <c r="N18" s="51"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A19" s="42">
+        <v>17</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="55">
+        <v>526251020790</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F19" s="56">
         <v>1211</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="G19" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="K2" s="31">
-        <v>44603</v>
-      </c>
-      <c r="L2" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="M2" s="31" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="21">
-        <v>2</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="23">
-        <v>526251024489</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1211</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="K3" s="31">
-        <v>44603</v>
-      </c>
-      <c r="L3" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="M3" s="31" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="21">
-        <v>3</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="23">
-        <v>526251452797</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1211</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="K4" s="31">
-        <v>44603</v>
-      </c>
-      <c r="L4" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="M4" s="31" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="21">
-        <v>4</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="23">
-        <v>526255917395</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1211</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="K5" s="31">
-        <v>44603</v>
-      </c>
-      <c r="L5" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="M5" s="31" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="21">
-        <v>5</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="23">
-        <v>526251193016</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1211</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="K6" s="31">
-        <v>44603</v>
-      </c>
-      <c r="L6" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="M6" s="31" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="21">
-        <v>6</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="23">
-        <v>526251579804</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1211</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="K7" s="31">
-        <v>44603</v>
-      </c>
-      <c r="L7" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="M7" s="31" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="21">
-        <v>7</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="23">
-        <v>526251201079</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="J8" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="K8" s="31">
-        <v>43872</v>
-      </c>
-      <c r="L8" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="M8" s="32" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="35">
-        <v>8</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="37">
-        <v>526251106286</v>
-      </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="39">
-        <v>1211</v>
-      </c>
-      <c r="G9" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="H9" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="J9" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="K9" s="33">
-        <v>44384</v>
-      </c>
-      <c r="L9" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="M9" s="27" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="21">
-        <v>9</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="23">
-        <v>526258372598</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1211</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="J10" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="21">
-        <v>10</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="23">
-        <v>526251531996</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1211</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="J11" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="21">
-        <v>11</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="23">
-        <v>526251259145</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="4">
-        <v>1211</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="J12" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="21">
-        <v>12</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="23">
-        <v>526251060168</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1211</v>
-      </c>
-      <c r="G13" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="J13" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="21">
-        <v>13</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="23">
-        <v>526251037317</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="4">
-        <v>1312</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="J14" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="21">
-        <v>14</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="23">
-        <v>526251342314</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="4">
-        <v>1211</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="J15" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="21">
-        <v>15</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="C16" s="30">
-        <v>526251020232</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="24">
-        <v>1312</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="J16" s="34" t="s">
+      <c r="I19" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="K19" s="51" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A17" s="21">
-        <v>16</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="23">
-        <v>526251059200</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="4">
-        <v>1211</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I17" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="J17" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="21">
-        <v>17</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="30">
-        <v>526251020790</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="28">
-        <v>1211</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I18" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="J18" s="34" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B19" s="29"/>
+      <c r="L19" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="M19" s="39">
+        <v>44647</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="B20" s="57"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="L23" s="33" t="s">
+        <v>112</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="O1:W1"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Embebido, PWA y Control de equipos
Embebido:
- Bug en la seguridad. Separación de la lectura directa del efecto hall.
- Se agregó arreglo de configuración
PWA:
- Mejoras en la UI
Control de equipos:
- Se agregó columna de configuración
</commit_message>
<xml_diff>
--- a/Control de equipos.xlsx
+++ b/Control de equipos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L03502024\Documents\GitHub\dta-agricola\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam\Documents\GitHub\dta-agricola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81ABBCB-1C7B-4E97-9ECD-6FF65599EA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D12255-5A57-419D-8755-2D18A8DC9CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="458" xr2:uid="{81E9D037-BE23-435E-B775-5A4C621A153A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" tabRatio="458" xr2:uid="{81E9D037-BE23-435E-B775-5A4C621A153A}"/>
   </bookViews>
   <sheets>
     <sheet name="Control de equipos" sheetId="8" r:id="rId1"/>
@@ -26,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="146">
   <si>
     <t>Equipo</t>
   </si>
@@ -448,6 +446,33 @@
   </si>
   <si>
     <t>Pv66 v0.2.4.220529 A</t>
+  </si>
+  <si>
+    <t>8952020020633586696</t>
+  </si>
+  <si>
+    <t>Pv66 v0.2.4.220626 A</t>
+  </si>
+  <si>
+    <t>{0, 3, 2, 12, 11, 1}</t>
+  </si>
+  <si>
+    <t>Configuración</t>
+  </si>
+  <si>
+    <t>{1, 2, 3, 12, 11, 1}</t>
+  </si>
+  <si>
+    <t>{0, 2, 3, 12, 11, 0}</t>
+  </si>
+  <si>
+    <t>{0, 3, 2, 12, 11, 0}</t>
+  </si>
+  <si>
+    <t>{0, 2, 3, 13, 12, 0}</t>
+  </si>
+  <si>
+    <t>{1, 2, 3, 12, 11, 0}</t>
   </si>
 </sst>
 </file>
@@ -552,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -807,9 +832,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1132,48 +1154,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07BF86A-6972-496C-8446-0DD77854D911}">
-  <dimension ref="A1:X23"/>
+  <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13:H16"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.08984375" style="33" customWidth="1"/>
-    <col min="2" max="2" width="21.36328125" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" style="33" customWidth="1"/>
-    <col min="5" max="7" width="11.54296875" style="33"/>
-    <col min="8" max="8" width="19.453125" style="33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.54296875" style="33" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.36328125" style="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.26953125" style="33" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.81640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.08984375" style="33" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="19.1796875" style="33" customWidth="1"/>
-    <col min="16" max="16" width="36.453125" style="53" customWidth="1"/>
-    <col min="17" max="24" width="12.1796875" style="37" customWidth="1"/>
-    <col min="25" max="16384" width="11.54296875" style="33"/>
+    <col min="1" max="1" width="5.140625" style="33" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="33" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11.5703125" style="33"/>
+    <col min="9" max="9" width="19.42578125" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="19.140625" style="33" customWidth="1"/>
+    <col min="17" max="17" width="60.28515625" style="53" customWidth="1"/>
+    <col min="18" max="25" width="12.140625" style="37" customWidth="1"/>
+    <col min="26" max="16384" width="11.5703125" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="P1" s="92" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q1" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="92"/>
-      <c r="R1" s="92"/>
-      <c r="S1" s="92"/>
-      <c r="T1" s="92"/>
-      <c r="U1" s="92"/>
-      <c r="V1" s="92"/>
-      <c r="W1" s="92"/>
-      <c r="X1" s="92"/>
-    </row>
-    <row r="2" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="91"/>
+      <c r="U1" s="91"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="91"/>
+      <c r="X1" s="91"/>
+      <c r="Y1" s="91"/>
+    </row>
+    <row r="2" spans="1:25" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
@@ -1187,67 +1210,70 @@
         <v>69</v>
       </c>
       <c r="E2" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="G2" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="H2" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="I2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="J2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="K2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="L2" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="M2" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="N2" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="O2" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="P2" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="P2" s="22" t="s">
+      <c r="Q2" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="Q2" s="19">
+      <c r="R2" s="19">
         <v>1</v>
       </c>
-      <c r="R2" s="19">
+      <c r="S2" s="19">
         <v>2</v>
       </c>
-      <c r="S2" s="19">
+      <c r="T2" s="19">
         <v>3</v>
       </c>
-      <c r="T2" s="19">
+      <c r="U2" s="19">
         <v>4</v>
       </c>
-      <c r="U2" s="19">
+      <c r="V2" s="19">
         <v>5</v>
       </c>
-      <c r="V2" s="19">
+      <c r="W2" s="19">
         <v>6</v>
       </c>
-      <c r="W2" s="19">
+      <c r="X2" s="19">
         <v>7</v>
       </c>
-      <c r="X2" s="19">
+      <c r="Y2" s="19">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="32" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23">
         <v>1</v>
       </c>
@@ -1260,41 +1286,41 @@
       <c r="D3" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="80"/>
+      <c r="F3" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="G3" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="G3" s="27">
+      <c r="H3" s="27">
         <v>1211</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="I3" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="J3" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="K3" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="L3" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="23"/>
-      <c r="M3" s="29" t="s">
+      <c r="M3" s="23"/>
+      <c r="N3" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="N3" s="30">
+      <c r="O3" s="30">
         <v>43872</v>
       </c>
-      <c r="O3" s="23" t="s">
+      <c r="P3" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="P3" s="31" t="s">
+      <c r="Q3" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="Q3" s="58"/>
       <c r="R3" s="58"/>
       <c r="S3" s="58"/>
       <c r="T3" s="58"/>
@@ -1302,8 +1328,9 @@
       <c r="V3" s="58"/>
       <c r="W3" s="58"/>
       <c r="X3" s="58"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y3" s="58"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="33">
         <v>2</v>
       </c>
@@ -1316,41 +1343,44 @@
       <c r="D4" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="G4" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="G4" s="36">
+      <c r="H4" s="36">
         <v>1211</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="I4" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="J4" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="33" t="s">
+      <c r="K4" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="K4" s="33" t="s">
+      <c r="L4" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="M4" s="39" t="s">
+      <c r="N4" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="N4" s="40">
+      <c r="O4" s="40">
         <v>44603</v>
       </c>
-      <c r="O4" s="33" t="s">
+      <c r="P4" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="P4" s="41" t="s">
+      <c r="Q4" s="41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="42">
         <v>3</v>
       </c>
@@ -1363,41 +1393,44 @@
       <c r="D5" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="F5" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="G5" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="G5" s="36">
+      <c r="H5" s="36">
         <v>1211</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="I5" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="J5" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="33" t="s">
+      <c r="K5" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="K5" s="33" t="s">
+      <c r="L5" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="M5" s="39" t="s">
+      <c r="N5" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="N5" s="40">
+      <c r="O5" s="40">
         <v>44603</v>
       </c>
-      <c r="O5" s="33" t="s">
+      <c r="P5" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="P5" s="41" t="s">
+      <c r="Q5" s="41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="33">
         <v>4</v>
       </c>
@@ -1410,41 +1443,44 @@
       <c r="D6" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="G6" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="G6" s="36">
+      <c r="H6" s="36">
         <v>1211</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="I6" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="J6" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="K6" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="K6" s="33" t="s">
+      <c r="L6" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="M6" s="39" t="s">
+      <c r="N6" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="N6" s="40">
+      <c r="O6" s="40">
         <v>44603</v>
       </c>
-      <c r="O6" s="33" t="s">
+      <c r="P6" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="P6" s="41" t="s">
+      <c r="Q6" s="41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="42">
         <v>5</v>
       </c>
@@ -1457,41 +1493,44 @@
       <c r="D7" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="G7" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="G7" s="36">
+      <c r="H7" s="36">
         <v>1211</v>
       </c>
-      <c r="H7" s="36" t="s">
+      <c r="I7" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="I7" s="38" t="s">
+      <c r="J7" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="33" t="s">
+      <c r="K7" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="K7" s="33" t="s">
+      <c r="L7" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="M7" s="39" t="s">
+      <c r="N7" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="N7" s="40">
+      <c r="O7" s="40">
         <v>44603</v>
       </c>
-      <c r="O7" s="33" t="s">
+      <c r="P7" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="P7" s="41" t="s">
+      <c r="Q7" s="41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="33">
         <v>6</v>
       </c>
@@ -1504,41 +1543,44 @@
       <c r="D8" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="G8" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="G8" s="36">
+      <c r="H8" s="36">
         <v>1211</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="I8" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="I8" s="38" t="s">
+      <c r="J8" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="33" t="s">
+      <c r="K8" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="K8" s="33" t="s">
+      <c r="L8" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="M8" s="39" t="s">
+      <c r="N8" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="N8" s="40">
+      <c r="O8" s="40">
         <v>44603</v>
       </c>
-      <c r="O8" s="33" t="s">
+      <c r="P8" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="P8" s="41" t="s">
+      <c r="Q8" s="41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="42">
         <v>7</v>
       </c>
@@ -1551,42 +1593,45 @@
       <c r="D9" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="G9" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="G9" s="36">
+      <c r="H9" s="36">
         <v>1211</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="I9" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="I9" s="38" t="s">
+      <c r="J9" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="42" t="s">
+      <c r="K9" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="K9" s="42" t="s">
+      <c r="L9" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="L9" s="42"/>
-      <c r="M9" s="39" t="s">
+      <c r="M9" s="42"/>
+      <c r="N9" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="N9" s="40">
+      <c r="O9" s="40">
         <v>44603</v>
       </c>
-      <c r="O9" s="33" t="s">
+      <c r="P9" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="P9" s="41" t="s">
+      <c r="Q9" s="41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="42" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="33">
         <v>8</v>
       </c>
@@ -1599,41 +1644,43 @@
       <c r="D10" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="46" t="s">
+      <c r="E10" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="F10" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="G10" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="G10" s="46">
+      <c r="H10" s="46">
         <v>1211</v>
       </c>
-      <c r="H10" s="90" t="s">
+      <c r="I10" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="I10" s="47" t="s">
+      <c r="J10" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="48" t="s">
+      <c r="K10" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="K10" s="48" t="s">
+      <c r="L10" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="L10" s="48"/>
-      <c r="M10" s="39" t="s">
+      <c r="M10" s="48"/>
+      <c r="N10" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="N10" s="49">
+      <c r="O10" s="49">
         <v>44384</v>
       </c>
-      <c r="O10" s="42" t="s">
+      <c r="P10" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="P10" s="50" t="s">
+      <c r="Q10" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="Q10" s="56"/>
       <c r="R10" s="56"/>
       <c r="S10" s="56"/>
       <c r="T10" s="56"/>
@@ -1641,8 +1688,9 @@
       <c r="V10" s="56"/>
       <c r="W10" s="56"/>
       <c r="X10" s="56"/>
-    </row>
-    <row r="11" spans="1:24" s="59" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Y10" s="56"/>
+    </row>
+    <row r="11" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="59">
         <v>9</v>
       </c>
@@ -1655,39 +1703,41 @@
       <c r="D11" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="62" t="s">
+      <c r="E11" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="62" t="s">
+      <c r="G11" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="G11" s="62">
+      <c r="H11" s="62">
         <v>1211</v>
       </c>
-      <c r="H11" s="73" t="s">
+      <c r="I11" s="73" t="s">
         <v>126</v>
       </c>
-      <c r="I11" s="63" t="s">
+      <c r="J11" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="64" t="s">
+      <c r="K11" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="K11" s="64" t="s">
+      <c r="L11" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="L11" s="64" t="s">
+      <c r="M11" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="M11" s="69" t="s">
+      <c r="N11" s="69" t="s">
         <v>128</v>
       </c>
-      <c r="N11" s="65">
+      <c r="O11" s="65">
         <v>44646</v>
       </c>
-      <c r="O11" s="64"/>
-      <c r="P11" s="74"/>
-      <c r="Q11" s="68"/>
+      <c r="P11" s="64"/>
+      <c r="Q11" s="74"/>
       <c r="R11" s="68"/>
       <c r="S11" s="68"/>
       <c r="T11" s="68"/>
@@ -1695,8 +1745,9 @@
       <c r="V11" s="68"/>
       <c r="W11" s="68"/>
       <c r="X11" s="68"/>
-    </row>
-    <row r="12" spans="1:24" s="59" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="Y11" s="68"/>
+    </row>
+    <row r="12" spans="1:25" s="59" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="59">
         <v>10</v>
       </c>
@@ -1709,39 +1760,41 @@
       <c r="D12" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="62" t="s">
+      <c r="E12" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="62" t="s">
+      <c r="G12" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="62">
+      <c r="H12" s="62">
         <v>1211</v>
       </c>
-      <c r="H12" s="73" t="s">
+      <c r="I12" s="73" t="s">
         <v>134</v>
       </c>
-      <c r="I12" s="63" t="s">
+      <c r="J12" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="64" t="s">
+      <c r="K12" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="K12" s="64" t="s">
+      <c r="L12" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="L12" s="64" t="s">
+      <c r="M12" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="M12" s="69" t="s">
+      <c r="N12" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="N12" s="69"/>
-      <c r="O12" s="64"/>
-      <c r="P12" s="75" t="s">
+      <c r="O12" s="69"/>
+      <c r="P12" s="64"/>
+      <c r="Q12" s="75" t="s">
         <v>125</v>
       </c>
-      <c r="Q12" s="68"/>
       <c r="R12" s="68"/>
       <c r="S12" s="68"/>
       <c r="T12" s="68"/>
@@ -1749,8 +1802,9 @@
       <c r="V12" s="68"/>
       <c r="W12" s="68"/>
       <c r="X12" s="68"/>
-    </row>
-    <row r="13" spans="1:24" s="59" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="Y12" s="68"/>
+    </row>
+    <row r="13" spans="1:25" s="59" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="59">
         <v>11</v>
       </c>
@@ -1763,66 +1817,69 @@
       <c r="D13" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="62" t="s">
+      <c r="E13" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="62" t="s">
+      <c r="G13" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="G13" s="62">
+      <c r="H13" s="62">
         <v>1211</v>
       </c>
-      <c r="H13" s="73" t="s">
+      <c r="I13" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="I13" s="63" t="s">
+      <c r="J13" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="64" t="s">
+      <c r="K13" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="K13" s="64" t="s">
+      <c r="L13" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="L13" s="64" t="s">
+      <c r="M13" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="M13" s="65" t="s">
+      <c r="N13" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="N13" s="65">
+      <c r="O13" s="65">
         <v>44662</v>
       </c>
-      <c r="O13" s="64"/>
-      <c r="P13" s="66" t="s">
+      <c r="P13" s="64"/>
+      <c r="Q13" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="Q13" s="67" t="s">
+      <c r="R13" s="67" t="s">
         <v>122</v>
-      </c>
-      <c r="R13" s="68" t="s">
-        <v>119</v>
       </c>
       <c r="S13" s="68" t="s">
         <v>119</v>
       </c>
       <c r="T13" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="U13" s="68" t="s">
         <v>118</v>
-      </c>
-      <c r="U13" s="68" t="s">
-        <v>57</v>
       </c>
       <c r="V13" s="68" t="s">
         <v>57</v>
       </c>
       <c r="W13" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="X13" s="68" t="s">
         <v>119</v>
       </c>
-      <c r="X13" s="68" t="s">
+      <c r="Y13" s="68" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:24" s="77" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" s="77" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="77">
         <v>12</v>
       </c>
@@ -1836,27 +1893,29 @@
         <v>72</v>
       </c>
       <c r="E14" s="80" t="s">
+        <v>142</v>
+      </c>
+      <c r="F14" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="80" t="s">
+      <c r="G14" s="80" t="s">
         <v>131</v>
       </c>
-      <c r="G14" s="80">
+      <c r="H14" s="80">
         <v>1211</v>
       </c>
-      <c r="H14" s="86" t="s">
+      <c r="I14" s="86" t="s">
         <v>126</v>
       </c>
-      <c r="I14" s="81" t="s">
+      <c r="J14" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="M14" s="82" t="s">
+      <c r="N14" s="82" t="s">
         <v>120</v>
       </c>
-      <c r="N14" s="82"/>
-      <c r="O14" s="83"/>
-      <c r="P14" s="84"/>
-      <c r="Q14" s="85"/>
+      <c r="O14" s="82"/>
+      <c r="P14" s="83"/>
+      <c r="Q14" s="84"/>
       <c r="R14" s="85"/>
       <c r="S14" s="85"/>
       <c r="T14" s="85"/>
@@ -1864,8 +1923,9 @@
       <c r="V14" s="85"/>
       <c r="W14" s="85"/>
       <c r="X14" s="85"/>
-    </row>
-    <row r="15" spans="1:24" s="77" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Y14" s="85"/>
+    </row>
+    <row r="15" spans="1:25" s="77" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="77">
         <v>13</v>
       </c>
@@ -1879,28 +1939,28 @@
         <v>72</v>
       </c>
       <c r="E15" s="80" t="s">
+        <v>142</v>
+      </c>
+      <c r="F15" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="80" t="s">
+      <c r="G15" s="80" t="s">
         <v>131</v>
       </c>
-      <c r="G15" s="80">
+      <c r="H15" s="80">
         <v>1211</v>
       </c>
-      <c r="H15" s="86" t="s">
+      <c r="I15" s="86" t="s">
         <v>135</v>
       </c>
-      <c r="I15" s="81" t="s">
+      <c r="J15" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="N15" s="87">
+      <c r="O15" s="87">
         <v>44646</v>
       </c>
-      <c r="O15" s="83"/>
-      <c r="P15" s="88"/>
-      <c r="Q15" s="85" t="s">
-        <v>123</v>
-      </c>
+      <c r="P15" s="83"/>
+      <c r="Q15" s="88"/>
       <c r="R15" s="85" t="s">
         <v>123</v>
       </c>
@@ -1916,14 +1976,17 @@
       <c r="V15" s="85" t="s">
         <v>123</v>
       </c>
-      <c r="W15" s="89" t="s">
+      <c r="W15" s="85" t="s">
+        <v>123</v>
+      </c>
+      <c r="X15" s="89" t="s">
         <v>124</v>
       </c>
-      <c r="X15" s="85" t="s">
+      <c r="Y15" s="85" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:24" s="59" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="59">
         <v>14</v>
       </c>
@@ -1936,39 +1999,41 @@
       <c r="D16" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="62" t="s">
+      <c r="E16" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="F16" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="62" t="s">
+      <c r="G16" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="G16" s="62">
+      <c r="H16" s="62">
         <v>1312</v>
       </c>
-      <c r="H16" s="73" t="s">
+      <c r="I16" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="I16" s="63" t="s">
+      <c r="J16" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="64" t="s">
+      <c r="K16" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="K16" s="64" t="s">
+      <c r="L16" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="L16" s="64" t="s">
+      <c r="M16" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="M16" s="69" t="s">
+      <c r="N16" s="69" t="s">
         <v>120</v>
       </c>
-      <c r="N16" s="65">
+      <c r="O16" s="65">
         <v>44646</v>
       </c>
-      <c r="O16" s="64"/>
-      <c r="P16" s="70"/>
-      <c r="Q16" s="68"/>
+      <c r="P16" s="64"/>
+      <c r="Q16" s="70"/>
       <c r="R16" s="68"/>
       <c r="S16" s="68"/>
       <c r="T16" s="68"/>
@@ -1976,8 +2041,9 @@
       <c r="V16" s="68"/>
       <c r="W16" s="68"/>
       <c r="X16" s="68"/>
-    </row>
-    <row r="17" spans="1:24" s="59" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Y16" s="68"/>
+    </row>
+    <row r="17" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="59">
         <v>15</v>
       </c>
@@ -1990,36 +2056,38 @@
       <c r="D17" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="62" t="s">
+      <c r="E17" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="F17" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="62" t="s">
+      <c r="G17" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="G17" s="68">
+      <c r="H17" s="68">
         <v>1312</v>
       </c>
-      <c r="H17" s="73" t="s">
+      <c r="I17" s="73" t="s">
         <v>133</v>
       </c>
-      <c r="I17" s="63" t="s">
+      <c r="J17" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="64" t="s">
+      <c r="K17" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="K17" s="64" t="s">
+      <c r="L17" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="L17" s="64" t="s">
+      <c r="M17" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="M17" s="65" t="s">
+      <c r="N17" s="65" t="s">
         <v>110</v>
       </c>
-      <c r="N17" s="69"/>
-      <c r="P17" s="72"/>
-      <c r="Q17" s="68"/>
+      <c r="O17" s="69"/>
+      <c r="Q17" s="72"/>
       <c r="R17" s="68"/>
       <c r="S17" s="68"/>
       <c r="T17" s="68"/>
@@ -2027,8 +2095,9 @@
       <c r="V17" s="68"/>
       <c r="W17" s="68"/>
       <c r="X17" s="68"/>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y17" s="68"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="33">
         <v>16</v>
       </c>
@@ -2041,39 +2110,42 @@
       <c r="D18" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="37" t="s">
+      <c r="E18" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="F18" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="G18" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="G18" s="36">
+      <c r="H18" s="36">
         <v>1211</v>
       </c>
-      <c r="H18" s="36" t="s">
+      <c r="I18" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="I18" s="38" t="s">
+      <c r="J18" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="51" t="s">
+      <c r="K18" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="K18" s="51" t="s">
+      <c r="L18" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="L18" s="51" t="s">
+      <c r="M18" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="M18" s="52" t="s">
+      <c r="N18" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="N18" s="39">
+      <c r="O18" s="39">
         <v>44647</v>
       </c>
-      <c r="O18" s="51"/>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="P18" s="51"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="42">
         <v>17</v>
       </c>
@@ -2086,38 +2158,44 @@
       <c r="D19" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="37" t="s">
+      <c r="E19" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="F19" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="37" t="s">
+      <c r="G19" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="G19" s="56">
+      <c r="H19" s="56">
         <v>1211</v>
       </c>
-      <c r="H19" s="36" t="s">
+      <c r="I19" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="I19" s="38" t="s">
+      <c r="J19" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="J19" s="37" t="s">
+      <c r="K19" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="K19" s="54" t="s">
+      <c r="L19" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="L19" s="51" t="s">
+      <c r="M19" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="M19" s="52" t="s">
+      <c r="N19" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="N19" s="39">
+      <c r="O19" s="39">
         <v>44647</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" s="33">
+        <v>18</v>
+      </c>
       <c r="B20" s="57" t="s">
         <v>129</v>
       </c>
@@ -2128,29 +2206,64 @@
         <v>72</v>
       </c>
       <c r="E20" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="F20" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="37" t="s">
+      <c r="G20" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="G20" s="37">
+      <c r="H20" s="37">
         <v>1211</v>
       </c>
-      <c r="H20" s="91" t="s">
+      <c r="I20" s="90" t="s">
         <v>126</v>
       </c>
-      <c r="I20" s="38" t="s">
+      <c r="J20" s="38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="M23" s="33" t="s">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21" s="42">
+        <v>19</v>
+      </c>
+      <c r="B21" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" s="76">
+        <v>526251020596</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="H21" s="37">
+        <v>1211</v>
+      </c>
+      <c r="I21" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="J21" s="38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="N23" s="33" t="s">
         <v>111</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="P1:X1"/>
+    <mergeCell ref="Q1:Y1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2169,22 +2282,22 @@
       <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2207,7 +2320,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2228,7 +2341,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2249,7 +2362,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2270,7 +2383,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2288,7 +2401,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2309,7 +2422,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2330,7 +2443,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2348,7 +2461,7 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2369,7 +2482,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2393,7 +2506,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2414,7 +2527,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2439,7 +2552,7 @@
       </c>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2460,14 +2573,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="2"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2484,7 +2597,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2501,7 +2614,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2533,16 +2646,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
@@ -2562,7 +2675,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -2582,7 +2695,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>20</v>
       </c>
@@ -2603,7 +2716,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -2626,7 +2739,7 @@
         <v>345.65371190683862</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
@@ -2649,7 +2762,7 @@
         <v>299.10009522643691</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
@@ -2672,7 +2785,7 @@
         <v>243.3192539009892</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
@@ -2695,7 +2808,7 @@
         <v>24.361651550915141</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
@@ -2718,7 +2831,7 @@
         <v>67.958809766553713</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
@@ -2741,7 +2854,7 @@
         <v>105.9883938172799</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -2764,7 +2877,7 @@
         <v>161.06125720466682</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
@@ -2787,7 +2900,7 @@
         <v>205.56089781590984</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>28407180</v>
       </c>
@@ -2807,7 +2920,7 @@
         <v>195.25884947744478</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <f>F7</f>
         <v>24.361651550915141</v>
@@ -2823,7 +2936,7 @@
         <v>299.10009522643691</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="15">
         <f>E7</f>
         <v>84.256470319224107</v>
@@ -2839,7 +2952,7 @@
         <v>358.99491399474584</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="C15" s="10" t="s">
         <v>22</v>
@@ -2851,7 +2964,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <f>F8</f>
         <v>67.958809766553713</v>
@@ -2878,7 +2991,7 @@
         <v>243.3192539009892</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="16"/>
       <c r="C17" s="10" t="s">
@@ -2891,7 +3004,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="15">
         <f>E9</f>
         <v>165.88321258558886</v>
@@ -2906,7 +3019,7 @@
         <v>265.45571658421881</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <f>F9</f>
         <v>105.9883938172799</v>
@@ -2934,17 +3047,17 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
@@ -2964,7 +3077,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -2990,7 +3103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>20</v>
       </c>
@@ -3022,7 +3135,7 @@
         <v>79.75958657020071</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -3053,7 +3166,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
@@ -3084,7 +3197,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
@@ -3126,7 +3239,7 @@
         <v>311.55235069652736</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
@@ -3157,7 +3270,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
@@ -3188,7 +3301,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
@@ -3219,7 +3332,7 @@
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -3261,7 +3374,7 @@
         <v>279.68743150639153</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
@@ -3303,7 +3416,7 @@
         <v>275.34248147520822</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>28407180</v>
       </c>
@@ -3343,7 +3456,7 @@
         <v>100.24537818567508</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <f>F7</f>
         <v>285.07125449016206</v>
@@ -3359,7 +3472,7 @@
         <v>285.07125449016206</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="15">
         <f>E7</f>
         <v>345.11346853390057</v>
@@ -3375,7 +3488,7 @@
         <v>345.11346853390057</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="C15" s="10" t="s">
         <v>22</v>
@@ -3387,7 +3500,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <f>F8</f>
         <v>285.07125449016206</v>
@@ -3414,7 +3527,7 @@
         <v>331.35274803111065</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="16"/>
       <c r="C17" s="10" t="s">
@@ -3427,7 +3540,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="15">
         <f>E9</f>
         <v>345.11346853390057</v>
@@ -3442,7 +3555,7 @@
         <v>355.0535648792515</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <f>F9</f>
         <v>285.07125449016206</v>

</xml_diff>

<commit_message>
Actualización del control de equipos
</commit_message>
<xml_diff>
--- a/Control de equipos.xlsx
+++ b/Control de equipos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam\Documents\GitHub\dta-agricola\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L03502024\Documents\GitHub\dta-agricola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D12255-5A57-419D-8755-2D18A8DC9CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB37E823-2690-4018-9E43-D4D701D2530F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" tabRatio="458" xr2:uid="{81E9D037-BE23-435E-B775-5A4C621A153A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="458" xr2:uid="{81E9D037-BE23-435E-B775-5A4C621A153A}"/>
   </bookViews>
   <sheets>
     <sheet name="Control de equipos" sheetId="8" r:id="rId1"/>
@@ -26,8 +26,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="146">
   <si>
     <t>Equipo</t>
   </si>
@@ -412,9 +415,6 @@
     <t>Baja</t>
   </si>
   <si>
-    <t>Límite máximo de 80% para evitar torcedura, debido a que el penúltimo motor es de Baja y no puede seguir el ritmo del último | Seguridad se corta constantemente y espera 3 min para conectarse nuevamente</t>
-  </si>
-  <si>
     <t>Pv66 v0.2.4.220414 A</t>
   </si>
   <si>
@@ -439,9 +439,6 @@
     <t>Pv66 v0.2.4.220501 A</t>
   </si>
   <si>
-    <t>Pv66 v0.2.4.220512 A</t>
-  </si>
-  <si>
     <t>Pv66 v0.2.4.220528 A</t>
   </si>
   <si>
@@ -473,6 +470,12 @@
   </si>
   <si>
     <t>{1, 2, 3, 12, 11, 0}</t>
+  </si>
+  <si>
+    <t>Batería</t>
+  </si>
+  <si>
+    <t>Sí</t>
   </si>
 </sst>
 </file>
@@ -577,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -789,9 +792,6 @@
     <xf numFmtId="14" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -816,9 +816,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -839,6 +836,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1154,49 +1169,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07BF86A-6972-496C-8446-0DD77854D911}">
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="33" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="33" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="11.5703125" style="33"/>
-    <col min="9" max="9" width="19.42578125" style="33" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.85546875" style="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" style="33" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" style="33" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" style="33" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.140625" style="33" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="19.140625" style="33" customWidth="1"/>
-    <col min="17" max="17" width="60.28515625" style="53" customWidth="1"/>
-    <col min="18" max="25" width="12.140625" style="37" customWidth="1"/>
-    <col min="26" max="16384" width="11.5703125" style="33"/>
+    <col min="1" max="1" width="5.1796875" style="33" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="33" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" style="33" customWidth="1"/>
+    <col min="7" max="7" width="7.54296875" style="33" customWidth="1"/>
+    <col min="8" max="8" width="8.36328125" style="33" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.453125" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.81640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" style="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.26953125" style="33" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.1796875" style="33" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="19.1796875" style="33" customWidth="1"/>
+    <col min="18" max="18" width="60.26953125" style="53" customWidth="1"/>
+    <col min="19" max="26" width="12.1796875" style="37" customWidth="1"/>
+    <col min="27" max="16384" width="11.54296875" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="Q1" s="91" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="R1" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="91"/>
-      <c r="S1" s="91"/>
-      <c r="T1" s="91"/>
-      <c r="U1" s="91"/>
-      <c r="V1" s="91"/>
-      <c r="W1" s="91"/>
-      <c r="X1" s="91"/>
-      <c r="Y1" s="91"/>
-    </row>
-    <row r="2" spans="1:25" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S1" s="89"/>
+      <c r="T1" s="89"/>
+      <c r="U1" s="89"/>
+      <c r="V1" s="89"/>
+      <c r="W1" s="89"/>
+      <c r="X1" s="89"/>
+      <c r="Y1" s="89"/>
+      <c r="Z1" s="89"/>
+    </row>
+    <row r="2" spans="1:26" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
@@ -1210,70 +1228,73 @@
         <v>69</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>140</v>
+        <v>2</v>
       </c>
       <c r="F2" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="R2" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="S2" s="19">
+        <v>1</v>
+      </c>
+      <c r="T2" s="19">
         <v>2</v>
       </c>
-      <c r="G2" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="19" t="s">
+      <c r="U2" s="19">
+        <v>3</v>
+      </c>
+      <c r="V2" s="19">
+        <v>4</v>
+      </c>
+      <c r="W2" s="19">
+        <v>5</v>
+      </c>
+      <c r="X2" s="19">
         <v>6</v>
       </c>
-      <c r="K2" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="M2" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="N2" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="P2" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q2" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="R2" s="19">
-        <v>1</v>
-      </c>
-      <c r="S2" s="19">
-        <v>2</v>
-      </c>
-      <c r="T2" s="19">
-        <v>3</v>
-      </c>
-      <c r="U2" s="19">
-        <v>4</v>
-      </c>
-      <c r="V2" s="19">
-        <v>5</v>
-      </c>
-      <c r="W2" s="19">
-        <v>6</v>
-      </c>
-      <c r="X2" s="19">
+      <c r="Y2" s="19">
         <v>7</v>
       </c>
-      <c r="Y2" s="19">
+      <c r="Z2" s="19">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="23">
         <v>1</v>
       </c>
@@ -1286,42 +1307,42 @@
       <c r="D3" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="80"/>
+      <c r="E3" s="27" t="s">
+        <v>68</v>
+      </c>
       <c r="F3" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="H3" s="27">
+        <v>130</v>
+      </c>
+      <c r="G3" s="27">
         <v>1211</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="H3" s="27"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="K3" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="L3" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="M3" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="M3" s="23"/>
-      <c r="N3" s="29" t="s">
+      <c r="N3" s="23"/>
+      <c r="O3" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="O3" s="30">
+      <c r="P3" s="30">
         <v>43872</v>
       </c>
-      <c r="P3" s="23" t="s">
+      <c r="Q3" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q3" s="31" t="s">
+      <c r="R3" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="R3" s="58"/>
       <c r="S3" s="58"/>
       <c r="T3" s="58"/>
       <c r="U3" s="58"/>
@@ -1329,8 +1350,9 @@
       <c r="W3" s="58"/>
       <c r="X3" s="58"/>
       <c r="Y3" s="58"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z3" s="58"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="33">
         <v>2</v>
       </c>
@@ -1343,44 +1365,45 @@
       <c r="D4" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="36" t="s">
-        <v>141</v>
+      <c r="E4" s="37" t="s">
+        <v>9</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="H4" s="36">
+        <v>130</v>
+      </c>
+      <c r="G4" s="36">
         <v>1211</v>
       </c>
+      <c r="H4" s="36"/>
       <c r="I4" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="J4" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="J4" s="38" t="s">
+      <c r="K4" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="33" t="s">
+      <c r="L4" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="L4" s="33" t="s">
+      <c r="M4" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="N4" s="39" t="s">
+      <c r="O4" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="O4" s="40">
+      <c r="P4" s="40">
         <v>44603</v>
       </c>
-      <c r="P4" s="33" t="s">
+      <c r="Q4" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="Q4" s="41" t="s">
+      <c r="R4" s="41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="42">
         <v>3</v>
       </c>
@@ -1393,44 +1416,45 @@
       <c r="D5" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="36" t="s">
-        <v>142</v>
+      <c r="E5" s="37" t="s">
+        <v>3</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="H5" s="36">
+        <v>130</v>
+      </c>
+      <c r="G5" s="36">
         <v>1211</v>
       </c>
+      <c r="H5" s="36"/>
       <c r="I5" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="J5" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="J5" s="38" t="s">
+      <c r="K5" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="33" t="s">
+      <c r="L5" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="L5" s="33" t="s">
+      <c r="M5" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="39" t="s">
+      <c r="O5" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="O5" s="40">
+      <c r="P5" s="40">
         <v>44603</v>
       </c>
-      <c r="P5" s="33" t="s">
+      <c r="Q5" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="Q5" s="41" t="s">
+      <c r="R5" s="41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="33">
         <v>4</v>
       </c>
@@ -1443,44 +1467,45 @@
       <c r="D6" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="36" t="s">
-        <v>142</v>
+      <c r="E6" s="37" t="s">
+        <v>3</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="H6" s="36">
+        <v>130</v>
+      </c>
+      <c r="G6" s="36">
         <v>1211</v>
       </c>
+      <c r="H6" s="36"/>
       <c r="I6" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="J6" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="K6" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="33" t="s">
+      <c r="L6" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="M6" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="N6" s="39" t="s">
+      <c r="O6" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="O6" s="40">
+      <c r="P6" s="40">
         <v>44603</v>
       </c>
-      <c r="P6" s="33" t="s">
+      <c r="Q6" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="Q6" s="41" t="s">
+      <c r="R6" s="41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="42">
         <v>5</v>
       </c>
@@ -1493,44 +1518,45 @@
       <c r="D7" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="36" t="s">
-        <v>142</v>
+      <c r="E7" s="37" t="s">
+        <v>3</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="H7" s="36">
+        <v>130</v>
+      </c>
+      <c r="G7" s="36">
         <v>1211</v>
       </c>
+      <c r="H7" s="36"/>
       <c r="I7" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="J7" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="J7" s="38" t="s">
+      <c r="K7" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="33" t="s">
+      <c r="L7" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="L7" s="33" t="s">
+      <c r="M7" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="N7" s="39" t="s">
+      <c r="O7" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="O7" s="40">
+      <c r="P7" s="40">
         <v>44603</v>
       </c>
-      <c r="P7" s="33" t="s">
+      <c r="Q7" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="Q7" s="41" t="s">
+      <c r="R7" s="41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="33">
         <v>6</v>
       </c>
@@ -1543,44 +1569,45 @@
       <c r="D8" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="36" t="s">
-        <v>142</v>
+      <c r="E8" s="37" t="s">
+        <v>3</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="H8" s="36">
+        <v>130</v>
+      </c>
+      <c r="G8" s="36">
         <v>1211</v>
       </c>
+      <c r="H8" s="36"/>
       <c r="I8" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="J8" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="J8" s="38" t="s">
+      <c r="K8" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="33" t="s">
+      <c r="L8" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="L8" s="33" t="s">
+      <c r="M8" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="N8" s="39" t="s">
+      <c r="O8" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="O8" s="40">
+      <c r="P8" s="40">
         <v>44603</v>
       </c>
-      <c r="P8" s="33" t="s">
+      <c r="Q8" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="Q8" s="41" t="s">
+      <c r="R8" s="41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="42">
         <v>7</v>
       </c>
@@ -1593,45 +1620,46 @@
       <c r="D9" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="36" t="s">
-        <v>142</v>
+      <c r="E9" s="37" t="s">
+        <v>3</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="H9" s="36">
+        <v>130</v>
+      </c>
+      <c r="G9" s="36">
         <v>1211</v>
       </c>
+      <c r="H9" s="36"/>
       <c r="I9" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="J9" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="J9" s="38" t="s">
+      <c r="K9" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="42" t="s">
+      <c r="L9" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="L9" s="42" t="s">
+      <c r="M9" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="M9" s="42"/>
-      <c r="N9" s="39" t="s">
+      <c r="N9" s="42"/>
+      <c r="O9" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="O9" s="40">
+      <c r="P9" s="40">
         <v>44603</v>
       </c>
-      <c r="P9" s="33" t="s">
+      <c r="Q9" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="Q9" s="41" t="s">
+      <c r="R9" s="41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="33">
         <v>8</v>
       </c>
@@ -1644,44 +1672,46 @@
       <c r="D10" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="F10" s="46" t="s">
+      <c r="E10" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="G10" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="H10" s="46">
+      <c r="F10" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="G10" s="46">
         <v>1211</v>
       </c>
-      <c r="I10" s="45" t="s">
-        <v>136</v>
-      </c>
-      <c r="J10" s="47" t="s">
+      <c r="H10" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="I10" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="J10" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="K10" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="48" t="s">
+      <c r="L10" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="L10" s="48" t="s">
+      <c r="M10" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="M10" s="48"/>
-      <c r="N10" s="39" t="s">
+      <c r="N10" s="48"/>
+      <c r="O10" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="O10" s="49">
+      <c r="P10" s="49">
         <v>44384</v>
       </c>
-      <c r="P10" s="42" t="s">
+      <c r="Q10" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="Q10" s="50" t="s">
+      <c r="R10" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="R10" s="56"/>
       <c r="S10" s="56"/>
       <c r="T10" s="56"/>
       <c r="U10" s="56"/>
@@ -1689,56 +1719,56 @@
       <c r="W10" s="56"/>
       <c r="X10" s="56"/>
       <c r="Y10" s="56"/>
-    </row>
-    <row r="11" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z10" s="56"/>
+    </row>
+    <row r="11" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="59">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B11" s="60" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="61">
-        <v>526258372598</v>
+        <v>82</v>
+      </c>
+      <c r="C11" s="71">
+        <v>526251020232</v>
       </c>
       <c r="D11" s="62" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="62" t="s">
+        <v>130</v>
+      </c>
+      <c r="G11" s="68">
+        <v>1312</v>
+      </c>
+      <c r="H11" s="68" t="s">
+        <v>145</v>
+      </c>
+      <c r="I11" s="62" t="s">
         <v>142</v>
       </c>
-      <c r="F11" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="62" t="s">
-        <v>131</v>
-      </c>
-      <c r="H11" s="62">
-        <v>1211</v>
-      </c>
-      <c r="I11" s="73" t="s">
-        <v>126</v>
-      </c>
-      <c r="J11" s="63" t="s">
+      <c r="J11" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="K11" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="64" t="s">
+      <c r="L11" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="L11" s="64" t="s">
-        <v>127</v>
-      </c>
       <c r="M11" s="64" t="s">
+        <v>94</v>
+      </c>
+      <c r="N11" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="N11" s="69" t="s">
-        <v>128</v>
-      </c>
-      <c r="O11" s="65">
-        <v>44646</v>
-      </c>
-      <c r="P11" s="64"/>
-      <c r="Q11" s="74"/>
-      <c r="R11" s="68"/>
+      <c r="O11" s="65" t="s">
+        <v>110</v>
+      </c>
+      <c r="P11" s="69"/>
+      <c r="R11" s="72"/>
       <c r="S11" s="68"/>
       <c r="T11" s="68"/>
       <c r="U11" s="68"/>
@@ -1746,358 +1776,379 @@
       <c r="W11" s="68"/>
       <c r="X11" s="68"/>
       <c r="Y11" s="68"/>
-    </row>
-    <row r="12" spans="1:25" s="59" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="59">
-        <v>10</v>
-      </c>
-      <c r="B12" s="60" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="61">
-        <v>526251531996</v>
-      </c>
-      <c r="D12" s="62" t="s">
+      <c r="Z11" s="68"/>
+    </row>
+    <row r="12" spans="1:26" s="76" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="76">
+        <v>13</v>
+      </c>
+      <c r="B12" s="77" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="78">
+        <v>526251342314</v>
+      </c>
+      <c r="D12" s="79" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="F12" s="62" t="s">
+      <c r="E12" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="62" t="s">
-        <v>131</v>
-      </c>
-      <c r="H12" s="62">
+      <c r="F12" s="79" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" s="79">
         <v>1211</v>
       </c>
-      <c r="I12" s="73" t="s">
-        <v>134</v>
-      </c>
-      <c r="J12" s="63" t="s">
+      <c r="H12" s="79" t="s">
+        <v>145</v>
+      </c>
+      <c r="I12" s="79" t="s">
+        <v>140</v>
+      </c>
+      <c r="J12" s="84" t="s">
+        <v>133</v>
+      </c>
+      <c r="K12" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="K12" s="64" t="s">
+      <c r="L12" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="L12" s="64" t="s">
+      <c r="M12" s="76" t="s">
         <v>89</v>
       </c>
-      <c r="M12" s="64" t="s">
-        <v>91</v>
-      </c>
-      <c r="N12" s="69" t="s">
+      <c r="O12" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="O12" s="69"/>
-      <c r="P12" s="64"/>
-      <c r="Q12" s="75" t="s">
-        <v>125</v>
-      </c>
-      <c r="R12" s="68"/>
-      <c r="S12" s="68"/>
-      <c r="T12" s="68"/>
-      <c r="U12" s="68"/>
-      <c r="V12" s="68"/>
-      <c r="W12" s="68"/>
-      <c r="X12" s="68"/>
-      <c r="Y12" s="68"/>
-    </row>
-    <row r="13" spans="1:25" s="59" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="P12" s="85">
+        <v>44646</v>
+      </c>
+      <c r="Q12" s="82"/>
+      <c r="R12" s="86"/>
+      <c r="S12" s="83" t="s">
+        <v>123</v>
+      </c>
+      <c r="T12" s="83" t="s">
+        <v>123</v>
+      </c>
+      <c r="U12" s="83" t="s">
+        <v>123</v>
+      </c>
+      <c r="V12" s="83" t="s">
+        <v>123</v>
+      </c>
+      <c r="W12" s="83" t="s">
+        <v>123</v>
+      </c>
+      <c r="X12" s="83" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y12" s="87" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z12" s="83" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="59">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="60" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" s="61">
-        <v>526251259145</v>
+        <v>526258372598</v>
       </c>
       <c r="D13" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="62" t="s">
+        <v>130</v>
+      </c>
+      <c r="G13" s="62">
+        <v>1211</v>
+      </c>
+      <c r="H13" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="I13" s="62" t="s">
+        <v>140</v>
+      </c>
+      <c r="J13" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="K13" s="63" t="s">
+        <v>34</v>
+      </c>
+      <c r="L13" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="M13" s="64" t="s">
+        <v>126</v>
+      </c>
+      <c r="N13" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="O13" s="69" t="s">
+        <v>127</v>
+      </c>
+      <c r="P13" s="65">
+        <v>44646</v>
+      </c>
+      <c r="Q13" s="64"/>
+      <c r="R13" s="74"/>
+      <c r="S13" s="68"/>
+      <c r="T13" s="68"/>
+      <c r="U13" s="68"/>
+      <c r="V13" s="68"/>
+      <c r="W13" s="68"/>
+      <c r="X13" s="68"/>
+      <c r="Y13" s="68"/>
+      <c r="Z13" s="68"/>
+    </row>
+    <row r="14" spans="1:26" s="59" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="59">
+        <v>11</v>
+      </c>
+      <c r="B14" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="61">
+        <v>526251259145</v>
+      </c>
+      <c r="D14" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="62" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" s="62">
+        <v>1211</v>
+      </c>
+      <c r="H14" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="I14" s="62" t="s">
+        <v>140</v>
+      </c>
+      <c r="J14" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="K14" s="63" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="M14" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="N14" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="O14" s="65" t="s">
+        <v>102</v>
+      </c>
+      <c r="P14" s="65">
+        <v>44662</v>
+      </c>
+      <c r="Q14" s="64"/>
+      <c r="R14" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="S14" s="67" t="s">
+        <v>122</v>
+      </c>
+      <c r="T14" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="U14" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="V14" s="68" t="s">
+        <v>118</v>
+      </c>
+      <c r="W14" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="X14" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y14" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z14" s="68" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="59">
+        <v>14</v>
+      </c>
+      <c r="B15" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="61">
+        <v>526251037317</v>
+      </c>
+      <c r="D15" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="62" t="s">
+        <v>130</v>
+      </c>
+      <c r="G15" s="62">
+        <v>1312</v>
+      </c>
+      <c r="H15" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="I15" s="62" t="s">
         <v>142</v>
       </c>
-      <c r="F13" s="62" t="s">
+      <c r="J15" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="K15" s="63" t="s">
+        <v>34</v>
+      </c>
+      <c r="L15" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="M15" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="N15" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="O15" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="P15" s="65">
+        <v>44646</v>
+      </c>
+      <c r="Q15" s="64"/>
+      <c r="R15" s="70"/>
+      <c r="S15" s="68"/>
+      <c r="T15" s="68"/>
+      <c r="U15" s="68"/>
+      <c r="V15" s="68"/>
+      <c r="W15" s="68"/>
+      <c r="X15" s="68"/>
+      <c r="Y15" s="68"/>
+      <c r="Z15" s="68"/>
+    </row>
+    <row r="16" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="42">
+        <v>10</v>
+      </c>
+      <c r="B16" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="90">
+        <v>526251531996</v>
+      </c>
+      <c r="D16" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="62" t="s">
-        <v>131</v>
-      </c>
-      <c r="H13" s="62">
+      <c r="F16" s="91" t="s">
+        <v>130</v>
+      </c>
+      <c r="G16" s="91">
         <v>1211</v>
       </c>
-      <c r="I13" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="J13" s="63" t="s">
+      <c r="H16" s="91" t="s">
+        <v>145</v>
+      </c>
+      <c r="I16" s="91" t="s">
+        <v>140</v>
+      </c>
+      <c r="J16" s="92" t="s">
+        <v>136</v>
+      </c>
+      <c r="K16" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="K13" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="L13" s="64" t="s">
-        <v>95</v>
-      </c>
-      <c r="M13" s="64" t="s">
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="N13" s="65" t="s">
-        <v>102</v>
-      </c>
-      <c r="O13" s="65">
-        <v>44662</v>
-      </c>
-      <c r="P13" s="64"/>
-      <c r="Q13" s="66" t="s">
-        <v>117</v>
-      </c>
-      <c r="R13" s="67" t="s">
-        <v>122</v>
-      </c>
-      <c r="S13" s="68" t="s">
-        <v>119</v>
-      </c>
-      <c r="T13" s="68" t="s">
-        <v>119</v>
-      </c>
-      <c r="U13" s="68" t="s">
-        <v>118</v>
-      </c>
-      <c r="V13" s="68" t="s">
-        <v>57</v>
-      </c>
-      <c r="W13" s="68" t="s">
-        <v>57</v>
-      </c>
-      <c r="X13" s="68" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y13" s="68" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" s="77" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="77">
+      <c r="O16" s="94"/>
+      <c r="P16" s="94"/>
+      <c r="Q16" s="54"/>
+      <c r="R16" s="95"/>
+      <c r="S16" s="56"/>
+      <c r="T16" s="56"/>
+      <c r="U16" s="56"/>
+      <c r="V16" s="56"/>
+      <c r="W16" s="56"/>
+      <c r="X16" s="56"/>
+      <c r="Y16" s="56"/>
+      <c r="Z16" s="56"/>
+    </row>
+    <row r="17" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="42">
         <v>12</v>
       </c>
-      <c r="B14" s="78" t="s">
+      <c r="B17" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="79">
+      <c r="C17" s="90">
         <v>526251060168</v>
       </c>
-      <c r="D14" s="80" t="s">
+      <c r="D17" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="80" t="s">
-        <v>142</v>
-      </c>
-      <c r="F14" s="80" t="s">
+      <c r="E17" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="80" t="s">
-        <v>131</v>
-      </c>
-      <c r="H14" s="80">
+      <c r="F17" s="91" t="s">
+        <v>130</v>
+      </c>
+      <c r="G17" s="91">
         <v>1211</v>
       </c>
-      <c r="I14" s="86" t="s">
-        <v>126</v>
-      </c>
-      <c r="J14" s="81" t="s">
+      <c r="H17" s="91" t="s">
+        <v>145</v>
+      </c>
+      <c r="I17" s="91" t="s">
+        <v>140</v>
+      </c>
+      <c r="J17" s="92" t="s">
+        <v>136</v>
+      </c>
+      <c r="K17" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="N14" s="82" t="s">
-        <v>120</v>
-      </c>
-      <c r="O14" s="82"/>
-      <c r="P14" s="83"/>
-      <c r="Q14" s="84"/>
-      <c r="R14" s="85"/>
-      <c r="S14" s="85"/>
-      <c r="T14" s="85"/>
-      <c r="U14" s="85"/>
-      <c r="V14" s="85"/>
-      <c r="W14" s="85"/>
-      <c r="X14" s="85"/>
-      <c r="Y14" s="85"/>
-    </row>
-    <row r="15" spans="1:25" s="77" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="77">
-        <v>13</v>
-      </c>
-      <c r="B15" s="78" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="79">
-        <v>526251342314</v>
-      </c>
-      <c r="D15" s="80" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="80" t="s">
-        <v>142</v>
-      </c>
-      <c r="F15" s="80" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="80" t="s">
-        <v>131</v>
-      </c>
-      <c r="H15" s="80">
-        <v>1211</v>
-      </c>
-      <c r="I15" s="86" t="s">
-        <v>135</v>
-      </c>
-      <c r="J15" s="81" t="s">
-        <v>34</v>
-      </c>
-      <c r="O15" s="87">
-        <v>44646</v>
-      </c>
-      <c r="P15" s="83"/>
-      <c r="Q15" s="88"/>
-      <c r="R15" s="85" t="s">
-        <v>123</v>
-      </c>
-      <c r="S15" s="85" t="s">
-        <v>123</v>
-      </c>
-      <c r="T15" s="85" t="s">
-        <v>123</v>
-      </c>
-      <c r="U15" s="85" t="s">
-        <v>123</v>
-      </c>
-      <c r="V15" s="85" t="s">
-        <v>123</v>
-      </c>
-      <c r="W15" s="85" t="s">
-        <v>123</v>
-      </c>
-      <c r="X15" s="89" t="s">
-        <v>124</v>
-      </c>
-      <c r="Y15" s="85" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="59">
-        <v>14</v>
-      </c>
-      <c r="B16" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="61">
-        <v>526251037317</v>
-      </c>
-      <c r="D16" s="62" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="F16" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="62" t="s">
-        <v>131</v>
-      </c>
-      <c r="H16" s="62">
-        <v>1312</v>
-      </c>
-      <c r="I16" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="J16" s="63" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="L16" s="64" t="s">
-        <v>97</v>
-      </c>
-      <c r="M16" s="64" t="s">
-        <v>96</v>
-      </c>
-      <c r="N16" s="69" t="s">
-        <v>120</v>
-      </c>
-      <c r="O16" s="65">
-        <v>44646</v>
-      </c>
-      <c r="P16" s="64"/>
-      <c r="Q16" s="70"/>
-      <c r="R16" s="68"/>
-      <c r="S16" s="68"/>
-      <c r="T16" s="68"/>
-      <c r="U16" s="68"/>
-      <c r="V16" s="68"/>
-      <c r="W16" s="68"/>
-      <c r="X16" s="68"/>
-      <c r="Y16" s="68"/>
-    </row>
-    <row r="17" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="59">
-        <v>15</v>
-      </c>
-      <c r="B17" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="71">
-        <v>526251020232</v>
-      </c>
-      <c r="D17" s="62" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="F17" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="62" t="s">
-        <v>131</v>
-      </c>
-      <c r="H17" s="68">
-        <v>1312</v>
-      </c>
-      <c r="I17" s="73" t="s">
-        <v>133</v>
-      </c>
-      <c r="J17" s="63" t="s">
-        <v>34</v>
-      </c>
-      <c r="K17" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="L17" s="64" t="s">
-        <v>94</v>
-      </c>
-      <c r="M17" s="64" t="s">
-        <v>93</v>
-      </c>
-      <c r="N17" s="65" t="s">
-        <v>110</v>
-      </c>
-      <c r="O17" s="69"/>
-      <c r="Q17" s="72"/>
-      <c r="R17" s="68"/>
-      <c r="S17" s="68"/>
-      <c r="T17" s="68"/>
-      <c r="U17" s="68"/>
-      <c r="V17" s="68"/>
-      <c r="W17" s="68"/>
-      <c r="X17" s="68"/>
-      <c r="Y17" s="68"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="O17" s="94"/>
+      <c r="P17" s="94"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="95"/>
+      <c r="S17" s="56"/>
+      <c r="T17" s="56"/>
+      <c r="U17" s="56"/>
+      <c r="V17" s="56"/>
+      <c r="W17" s="56"/>
+      <c r="X17" s="56"/>
+      <c r="Y17" s="56"/>
+      <c r="Z17" s="56"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" s="33">
         <v>16</v>
       </c>
@@ -2110,42 +2161,43 @@
       <c r="D18" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="36" t="s">
-        <v>145</v>
+      <c r="E18" s="37" t="s">
+        <v>121</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="G18" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="H18" s="36">
+        <v>130</v>
+      </c>
+      <c r="G18" s="36">
         <v>1211</v>
       </c>
+      <c r="H18" s="36"/>
       <c r="I18" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="J18" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="J18" s="38" t="s">
+      <c r="K18" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="K18" s="51" t="s">
+      <c r="L18" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="L18" s="51" t="s">
+      <c r="M18" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="M18" s="51" t="s">
+      <c r="N18" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="N18" s="52" t="s">
+      <c r="O18" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="O18" s="39">
+      <c r="P18" s="39">
         <v>44647</v>
       </c>
-      <c r="P18" s="51"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q18" s="51"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" s="42">
         <v>17</v>
       </c>
@@ -2158,112 +2210,115 @@
       <c r="D19" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="36" t="s">
-        <v>145</v>
+      <c r="E19" s="37" t="s">
+        <v>9</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="H19" s="56">
+        <v>130</v>
+      </c>
+      <c r="G19" s="56">
         <v>1211</v>
       </c>
+      <c r="H19" s="56"/>
       <c r="I19" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="J19" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="J19" s="38" t="s">
+      <c r="K19" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="37" t="s">
+      <c r="L19" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="L19" s="54" t="s">
+      <c r="M19" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="M19" s="51" t="s">
+      <c r="N19" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="N19" s="52" t="s">
+      <c r="O19" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="O19" s="39">
+      <c r="P19" s="39">
         <v>44647</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" s="33">
         <v>18</v>
       </c>
       <c r="B20" s="57" t="s">
-        <v>129</v>
-      </c>
-      <c r="C20" s="76">
+        <v>128</v>
+      </c>
+      <c r="C20" s="75">
         <v>526251020642</v>
       </c>
       <c r="D20" s="36" t="s">
         <v>72</v>
       </c>
       <c r="E20" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="F20" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="H20" s="37">
+      <c r="F20" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="G20" s="37">
         <v>1211</v>
       </c>
-      <c r="I20" s="90" t="s">
-        <v>126</v>
-      </c>
-      <c r="J20" s="38" t="s">
+      <c r="H20" s="37"/>
+      <c r="I20" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="J20" s="88" t="s">
+        <v>125</v>
+      </c>
+      <c r="K20" s="38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" s="42">
         <v>19</v>
       </c>
       <c r="B21" s="57" t="s">
-        <v>137</v>
-      </c>
-      <c r="C21" s="76">
+        <v>135</v>
+      </c>
+      <c r="C21" s="75">
         <v>526251020596</v>
       </c>
       <c r="D21" s="36" t="s">
         <v>72</v>
       </c>
       <c r="E21" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="F21" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="H21" s="37">
+      <c r="F21" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="G21" s="37">
         <v>1211</v>
       </c>
-      <c r="I21" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="J21" s="38" t="s">
+      <c r="H21" s="37"/>
+      <c r="I21" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="J21" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="K21" s="38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="N23" s="33" t="s">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="O23" s="33" t="s">
         <v>111</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="Q1:Y1"/>
+    <mergeCell ref="R1:Z1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2282,22 +2337,22 @@
       <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2320,7 +2375,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2341,7 +2396,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2362,7 +2417,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2383,7 +2438,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2401,7 +2456,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2422,7 +2477,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2443,7 +2498,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2461,7 +2516,7 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2482,7 +2537,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2506,7 +2561,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2527,7 +2582,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2552,7 +2607,7 @@
       </c>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2573,14 +2628,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="2"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2597,7 +2652,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2614,7 +2669,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2646,16 +2701,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
@@ -2675,7 +2730,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -2695,7 +2750,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>20</v>
       </c>
@@ -2716,7 +2771,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -2739,7 +2794,7 @@
         <v>345.65371190683862</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
@@ -2762,7 +2817,7 @@
         <v>299.10009522643691</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
@@ -2785,7 +2840,7 @@
         <v>243.3192539009892</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
@@ -2808,7 +2863,7 @@
         <v>24.361651550915141</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
@@ -2831,7 +2886,7 @@
         <v>67.958809766553713</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
@@ -2854,7 +2909,7 @@
         <v>105.9883938172799</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -2877,7 +2932,7 @@
         <v>161.06125720466682</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
@@ -2900,7 +2955,7 @@
         <v>205.56089781590984</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>28407180</v>
       </c>
@@ -2920,7 +2975,7 @@
         <v>195.25884947744478</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <f>F7</f>
         <v>24.361651550915141</v>
@@ -2936,7 +2991,7 @@
         <v>299.10009522643691</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B14" s="15">
         <f>E7</f>
         <v>84.256470319224107</v>
@@ -2952,7 +3007,7 @@
         <v>358.99491399474584</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="C15" s="10" t="s">
         <v>22</v>
@@ -2964,7 +3019,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14">
         <f>F8</f>
         <v>67.958809766553713</v>
@@ -2991,7 +3046,7 @@
         <v>243.3192539009892</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="16"/>
       <c r="C17" s="10" t="s">
@@ -3004,7 +3059,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B18" s="15">
         <f>E9</f>
         <v>165.88321258558886</v>
@@ -3019,7 +3074,7 @@
         <v>265.45571658421881</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <f>F9</f>
         <v>105.9883938172799</v>
@@ -3047,17 +3102,17 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
@@ -3077,7 +3132,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -3103,7 +3158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>20</v>
       </c>
@@ -3135,7 +3190,7 @@
         <v>79.75958657020071</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -3166,7 +3221,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
@@ -3197,7 +3252,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
@@ -3239,7 +3294,7 @@
         <v>311.55235069652736</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
@@ -3270,7 +3325,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
@@ -3301,7 +3356,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
@@ -3332,7 +3387,7 @@
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -3374,7 +3429,7 @@
         <v>279.68743150639153</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
@@ -3416,7 +3471,7 @@
         <v>275.34248147520822</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>28407180</v>
       </c>
@@ -3456,7 +3511,7 @@
         <v>100.24537818567508</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <f>F7</f>
         <v>285.07125449016206</v>
@@ -3472,7 +3527,7 @@
         <v>285.07125449016206</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14" s="15">
         <f>E7</f>
         <v>345.11346853390057</v>
@@ -3488,7 +3543,7 @@
         <v>345.11346853390057</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="C15" s="10" t="s">
         <v>22</v>
@@ -3500,7 +3555,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14">
         <f>F8</f>
         <v>285.07125449016206</v>
@@ -3527,7 +3582,7 @@
         <v>331.35274803111065</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="16"/>
       <c r="C17" s="10" t="s">
@@ -3540,7 +3595,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B18" s="15">
         <f>E9</f>
         <v>345.11346853390057</v>
@@ -3555,7 +3610,7 @@
         <v>355.0535648792515</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <f>F9</f>
         <v>285.07125449016206</v>

</xml_diff>